<commit_message>
docs: update sprint backlog
</commit_message>
<xml_diff>
--- a/docs/PMA_Sprint_backlog (Projekti_2025).xlsx
+++ b/docs/PMA_Sprint_backlog (Projekti_2025).xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93D1490-B719-4FE5-8DEA-05E6EDBED3EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="780" windowWidth="14805" windowHeight="8025"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1. (-08.1.)" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
   <si>
     <t>Product backlog stavka</t>
   </si>
@@ -37,21 +38,12 @@
     <t>Sprint zadatak (sprint task)</t>
   </si>
   <si>
-    <t>Postavljanje Expo projekta i Firebase konfiguracije</t>
-  </si>
-  <si>
     <t>4h</t>
   </si>
   <si>
     <t>Leo Petrović</t>
   </si>
   <si>
-    <t>Inicijalizacija projekta i integracija Firebase-a za autentifikaciju.</t>
-  </si>
-  <si>
-    <t>Implementacija ruta i osnovnog UI-a</t>
-  </si>
-  <si>
     <t>3h</t>
   </si>
   <si>
@@ -61,40 +53,55 @@
     <t>Dragan Arapović</t>
   </si>
   <si>
-    <t>Omogućiti prijavu korisnika pomoću Firebase-a.</t>
-  </si>
-  <si>
-    <t>Dodati rute za prijavu, registraciju, te osnovne stilove.</t>
-  </si>
-  <si>
     <t>Implementacija registracije korisnika</t>
   </si>
   <si>
     <t>Mate Marić</t>
   </si>
   <si>
-    <t>Dodati funkcionalnost registracije pomoću Firebase-a.</t>
-  </si>
-  <si>
     <t>Postavljanje route guardova</t>
   </si>
   <si>
     <t>2h</t>
   </si>
   <si>
-    <t>Dodati zaštitu ruta za prijavljene korisnike.</t>
-  </si>
-  <si>
     <t>Testiranje funkcionalnosti prijave i registracije.</t>
   </si>
   <si>
     <t>Provjeriti ispravnost ključnih funkcionalnosti.</t>
+  </si>
+  <si>
+    <t>Inicijalizacija I konfiguracija projekta</t>
+  </si>
+  <si>
+    <t>Implementacija navigacije i osnovnog UI-a</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>Konfigurirati rute za prijavu i registraciju, implementirati neke osnovne komponente, teme, boje, itd.</t>
+  </si>
+  <si>
+    <t>Omogućiti prijavu korisnika pomoću Supabase-a.</t>
+  </si>
+  <si>
+    <t>Dodati funkcionalnost registracije pomoću Supabase-a.</t>
+  </si>
+  <si>
+    <t>5h</t>
+  </si>
+  <si>
+    <t>Dodati zaštitu ruta za prijavljene korisnike koristeći Supabase realtime auth.</t>
+  </si>
+  <si>
+    <t>Inicijaliziranje Expo projekta, stvaranje novog Supabase projekta, i spajanje na Supabase.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -331,15 +338,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -351,6 +349,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -370,9 +377,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -410,7 +417,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -482,7 +489,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -655,11 +662,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -698,114 +705,118 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="16"/>
-    </row>
-    <row r="3" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
       <c r="B3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="15"/>
+      <c r="B4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7" t="s">
+      <c r="F4" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="B5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>8</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>11</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
       <c r="B7" s="8" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>23</v>
+      <c r="A8" s="15"/>
+      <c r="B8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="15"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -813,7 +824,7 @@
       <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -821,7 +832,7 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -829,7 +840,7 @@
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -837,7 +848,7 @@
       <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -845,7 +856,7 @@
       <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -853,7 +864,7 @@
       <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -861,7 +872,7 @@
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -869,7 +880,7 @@
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -877,7 +888,7 @@
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -961,7 +972,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1005,7 +1016,7 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -1013,7 +1024,7 @@
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -1021,7 +1032,7 @@
       <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -1029,7 +1040,7 @@
       <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -1037,7 +1048,7 @@
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -1045,7 +1056,7 @@
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -1053,7 +1064,7 @@
       <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -1061,7 +1072,7 @@
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -1069,7 +1080,7 @@
       <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -1077,7 +1088,7 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -1093,7 +1104,7 @@
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -1101,7 +1112,7 @@
       <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -1109,7 +1120,7 @@
       <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -1117,7 +1128,7 @@
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -1125,7 +1136,7 @@
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -1133,7 +1144,7 @@
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -1141,7 +1152,7 @@
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -1149,7 +1160,7 @@
       <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -1157,7 +1168,7 @@
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+      <c r="A22" s="15"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -1165,7 +1176,7 @@
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -1183,7 +1194,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1227,7 +1238,7 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -1235,7 +1246,7 @@
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -1243,7 +1254,7 @@
       <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -1251,7 +1262,7 @@
       <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -1259,7 +1270,7 @@
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -1267,7 +1278,7 @@
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -1275,7 +1286,7 @@
       <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -1283,7 +1294,7 @@
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -1291,7 +1302,7 @@
       <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -1299,7 +1310,7 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -1315,7 +1326,7 @@
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -1323,7 +1334,7 @@
       <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -1331,7 +1342,7 @@
       <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -1339,7 +1350,7 @@
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -1347,7 +1358,7 @@
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -1355,7 +1366,7 @@
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -1363,7 +1374,7 @@
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -1371,7 +1382,7 @@
       <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -1379,7 +1390,7 @@
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+      <c r="A22" s="15"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -1387,7 +1398,7 @@
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -1405,7 +1416,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1451,7 +1462,7 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -1459,7 +1470,7 @@
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -1467,7 +1478,7 @@
       <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -1475,7 +1486,7 @@
       <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -1483,7 +1494,7 @@
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -1491,7 +1502,7 @@
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -1499,7 +1510,7 @@
       <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -1507,7 +1518,7 @@
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -1515,7 +1526,7 @@
       <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -1523,7 +1534,7 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -1539,7 +1550,7 @@
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -1547,7 +1558,7 @@
       <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -1555,7 +1566,7 @@
       <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -1563,7 +1574,7 @@
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -1571,7 +1582,7 @@
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -1579,7 +1590,7 @@
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -1587,7 +1598,7 @@
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -1595,7 +1606,7 @@
       <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -1603,7 +1614,7 @@
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+      <c r="A22" s="15"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -1611,7 +1622,7 @@
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>

</xml_diff>